<commit_message>
feat: Implement monthly minimum hours, improve fairness algorithm, and enhance validation report
</commit_message>
<xml_diff>
--- a/schedule_export.xlsx
+++ b/schedule_export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,12 +491,17 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>A2C</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>A2C</t>
+          <t>B1\</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -513,39 +518,40 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>吳靜蕙, 陳美娜</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>林宏諺</t>
-        </is>
-      </c>
+          <t>陳美娜</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>黃素珠</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>鄭靜慧</t>
+          <t>林群皓</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>黃素珠</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>李巧如</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr"/>
+          <t>鄭靜慧</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>陳昱勳</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
-          <t>陳怡芯, 賴桂蘭</t>
+          <t>吳靜蕙, 賴桂蘭</t>
         </is>
       </c>
       <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -560,39 +566,40 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>林群皓, 黃素珠</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>陳彥銘</t>
-        </is>
-      </c>
+          <t>陳美娜</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>黃素珠</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>吳誼婷</t>
+          <t>陳怡芯</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>黃榮壹</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>賴桂蘭</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr"/>
+          <t>陳彥銘</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>林宏諺</t>
+        </is>
+      </c>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>陳昱勳, 楊依如</t>
+          <t>吳誼婷, 楊依如</t>
         </is>
       </c>
       <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -607,39 +614,40 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>鄭靜慧, 賴桂蘭</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
+          <t>陳美娜</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>賴桂蘭</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
         <is>
           <t>陳怡芯</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>吳靜蕙</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>陳美娜</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>林宏諺</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr"/>
+          <t>林群皓</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>鄭靜慧</t>
+        </is>
+      </c>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
-          <t>李巧如, 楊依如</t>
+          <t>李巧如, 黃素珠</t>
         </is>
       </c>
       <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -654,15 +662,15 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>吳誼婷, 黃素珠</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>李巧如</t>
-        </is>
-      </c>
+          <t>陳美娜</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>楊依如</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
           <t>林群皓</t>
@@ -674,19 +682,20 @@
           <t>陳昱勳</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>陳彥銘</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>吳靜蕙</t>
+        </is>
+      </c>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
-          <t>黃榮壹, 陳美娜</t>
+          <t>陳彥銘, 賴桂蘭</t>
         </is>
       </c>
       <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -701,15 +710,15 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>林宏諺, 賴桂蘭</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>楊依如</t>
-        </is>
-      </c>
+          <t>陳美娜</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>黃素珠</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
           <t>陳昱勳</t>
@@ -718,22 +727,23 @@
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
-          <t>陳怡芯</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>吳靜蕙</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr"/>
+          <t>林宏諺</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>吳誼婷</t>
+        </is>
+      </c>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>陳彥銘, 陳美娜</t>
+          <t>陳怡芯, 楊依如</t>
         </is>
       </c>
       <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -748,39 +758,40 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>陳怡芯, 黃素珠</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>吳靜蕙</t>
-        </is>
-      </c>
+          <t>陳美娜</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>賴桂蘭</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>林宏諺</t>
+          <t>林群皓</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
-          <t>鄭靜慧</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>林群皓</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr"/>
+          <t>李巧如</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>陳彥銘</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
-          <t>黃榮壹, 楊依如</t>
+          <t>林宏諺, 黃素珠</t>
         </is>
       </c>
       <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -793,20 +804,16 @@
           <t>Wed</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>陳昱勳, 賴桂蘭</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>林群皓</t>
-        </is>
-      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>楊依如</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>陳怡芯</t>
+          <t>陳昱勳</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
@@ -815,19 +822,20 @@
           <t>吳誼婷</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>黃榮壹</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>鄭靜慧</t>
+        </is>
+      </c>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
-          <t>鄭靜慧, 陳美娜</t>
+          <t>李巧如, 賴桂蘭</t>
         </is>
       </c>
       <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -842,32 +850,32 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>黃榮壹, 黃素珠</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>鄭靜慧</t>
-        </is>
-      </c>
+          <t>陳美娜</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>黃素珠</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>賴桂蘭</t>
+          <t>林群皓</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
-          <t>陳彥銘</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>陳昱勳</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr"/>
+          <t>吳靜蕙</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>林宏諺</t>
+        </is>
+      </c>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
@@ -875,6 +883,7 @@
         </is>
       </c>
       <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -889,39 +898,40 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>陳彥銘, 賴桂蘭</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>吳誼婷</t>
-        </is>
-      </c>
+          <t>陳美娜</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>賴桂蘭</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>黃素珠</t>
+          <t>陳昱勳</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
-          <t>李巧如</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
           <t>陳怡芯</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>陳彥銘</t>
+        </is>
+      </c>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr">
         <is>
-          <t>林群皓, 陳美娜</t>
+          <t>吳靜蕙, 黃素珠</t>
         </is>
       </c>
       <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -936,39 +946,40 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>林宏諺, 黃素珠</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>陳昱勳</t>
-        </is>
-      </c>
+          <t>陳美娜</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>楊依如</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>黃榮壹</t>
+          <t>林群皓</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t>吳靜蕙</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
           <t>鄭靜慧</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>吳誼婷</t>
+        </is>
+      </c>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr">
         <is>
-          <t>李巧如, 楊依如</t>
+          <t>陳怡芯, 賴桂蘭</t>
         </is>
       </c>
       <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -983,39 +994,40 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>陳彥銘, 賴桂蘭</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>吳誼婷</t>
-        </is>
-      </c>
+          <t>陳美娜</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>黃素珠</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>吳靜蕙</t>
+          <t>陳昱勳</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
         <is>
-          <t>林宏諺</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>楊依如</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr"/>
+          <t>李巧如</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>吳靜蕙</t>
+        </is>
+      </c>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr">
         <is>
-          <t>林群皓, 陳美娜</t>
+          <t>鄭靜慧, 楊依如</t>
         </is>
       </c>
       <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1030,39 +1042,40 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>鄭靜慧, 楊依如</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>李巧如</t>
-        </is>
-      </c>
+          <t>陳美娜</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>賴桂蘭</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>陳彥銘</t>
+          <t>林群皓</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
-          <t>林群皓</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>吳誼婷</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr"/>
+          <t>林宏諺</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>陳彥銘</t>
+        </is>
+      </c>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr">
         <is>
-          <t>陳怡芯, 陳美娜</t>
+          <t>李巧如, 黃素珠</t>
         </is>
       </c>
       <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1077,39 +1090,40 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>黃榮壹, 楊依如</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr">
+          <t>陳美娜</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>楊依如</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
         <is>
           <t>林宏諺</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>黃素珠</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
-          <t>賴桂蘭</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>吳靜蕙</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr"/>
+          <t>陳怡芯</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>鄭靜慧</t>
+        </is>
+      </c>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
-          <t>陳昱勳, 陳美娜</t>
+          <t>陳昱勳, 賴桂蘭</t>
         </is>
       </c>
       <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1122,41 +1136,38 @@
           <t>Wed</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>林群皓, 楊依如</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>陳美娜</t>
-        </is>
-      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>黃素珠</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>鄭靜慧</t>
+          <t>陳怡芯</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
-          <t>李巧如</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>黃素珠</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr"/>
+          <t>陳彥銘</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>吳誼婷</t>
+        </is>
+      </c>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
-          <t>吳誼婷, 賴桂蘭</t>
+          <t>林群皓, 楊依如</t>
         </is>
       </c>
       <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1171,39 +1182,40 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>李巧如, 楊依如</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr">
+          <t>陳美娜</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
         <is>
           <t>賴桂蘭</t>
         </is>
       </c>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>黃榮壹</t>
+          <t>陳彥銘</t>
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr">
         <is>
+          <t>吳靜蕙</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr">
+        <is>
           <t>陳昱勳</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>陳美娜</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr">
         <is>
-          <t>陳怡芯, 黃素珠</t>
+          <t>林宏諺, 黃素珠</t>
         </is>
       </c>
       <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1218,39 +1230,40 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>吳靜蕙, 陳美娜</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr">
+          <t>陳美娜</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>楊依如</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
         <is>
           <t>陳怡芯</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>李巧如</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
-          <t>陳彥銘</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>林宏諺</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr"/>
+          <t>李巧如</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>鄭靜慧</t>
+        </is>
+      </c>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr">
         <is>
-          <t>陳昱勳, 黃素珠</t>
+          <t>吳靜蕙, 賴桂蘭</t>
         </is>
       </c>
       <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1265,39 +1278,40 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>李巧如, 楊依如</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr">
+          <t>陳美娜</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
         <is>
           <t>黃素珠</t>
         </is>
       </c>
+      <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr">
         <is>
-          <t>林群皓</t>
+          <t>陳彥銘</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
         <is>
-          <t>鄭靜慧</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>黃榮壹</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr"/>
+          <t>吳誼婷</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>林宏諺</t>
+        </is>
+      </c>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr">
         <is>
-          <t>陳彥銘, 賴桂蘭</t>
+          <t>李巧如, 楊依如</t>
         </is>
       </c>
       <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1312,39 +1326,40 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>吳靜蕙, 陳美娜</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>黃榮壹</t>
-        </is>
-      </c>
+          <t>陳美娜</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>賴桂蘭</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
-          <t>林宏諺</t>
+          <t>陳怡芯</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
-          <t>楊依如</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>吳誼婷</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr"/>
+          <t>林群皓</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>吳靜蕙</t>
+        </is>
+      </c>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr">
         <is>
-          <t>鄭靜慧, 黃素珠</t>
+          <t>吳誼婷, 黃素珠</t>
         </is>
       </c>
       <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1359,32 +1374,32 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>吳誼婷, 陳美娜</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>陳昱勳</t>
-        </is>
-      </c>
+          <t>陳美娜</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>楊依如</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>楊依如</t>
+          <t>林群皓</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
         <is>
-          <t>陳怡芯</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>林群皓</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr"/>
+          <t>鄭靜慧</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>陳昱勳</t>
+        </is>
+      </c>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr">
         <is>
@@ -1392,6 +1407,7 @@
         </is>
       </c>
       <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1406,39 +1422,40 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>陳怡芯, 陳美娜</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>陳彥銘</t>
-        </is>
-      </c>
+          <t>陳美娜</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>黃素珠</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>吳誼婷</t>
+          <t>鄭靜慧</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
         <is>
-          <t>吳靜蕙</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>陳昱勳</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr"/>
+          <t>李巧如</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>林宏諺</t>
+        </is>
+      </c>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr">
         <is>
-          <t>林群皓, 黃素珠</t>
+          <t>陳怡芯, 楊依如</t>
         </is>
       </c>
       <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1451,41 +1468,38 @@
           <t>Wed</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>陳昱勳, 楊依如</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>吳靜蕙</t>
-        </is>
-      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>賴桂蘭</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>陳美娜</t>
+          <t>鄭靜慧</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr">
         <is>
-          <t>林宏諺</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>李巧如</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr"/>
+          <t>陳昱勳</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>吳靜蕙</t>
+        </is>
+      </c>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr">
         <is>
-          <t>鄭靜慧, 賴桂蘭</t>
+          <t>李巧如, 黃素珠</t>
         </is>
       </c>
       <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1500,39 +1514,40 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>林宏諺, 陳美娜</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>鄭靜慧</t>
-        </is>
-      </c>
+          <t>賴桂蘭</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>楊依如</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>陳怡芯</t>
+          <t>陳昱勳</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr">
         <is>
-          <t>林群皓</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
+          <t>吳誼婷</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr">
         <is>
           <t>陳彥銘</t>
         </is>
       </c>
-      <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr">
         <is>
-          <t>黃榮壹, 黃素珠</t>
+          <t>林群皓, 陳美娜</t>
         </is>
       </c>
       <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1547,39 +1562,40 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>吳誼婷, 楊依如</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>林群皓</t>
-        </is>
-      </c>
+          <t>賴桂蘭</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>陳美娜</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
-          <t>陳昱勳</t>
+          <t>鄭靜慧</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr">
         <is>
-          <t>黃榮壹</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>陳怡芯</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr"/>
+          <t>林宏諺</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>吳靜蕙</t>
+        </is>
+      </c>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr">
         <is>
-          <t>李巧如, 賴桂蘭</t>
+          <t>吳誼婷, 楊依如</t>
         </is>
       </c>
       <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1594,39 +1610,40 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>黃榮壹, 陳美娜</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr">
-        <is>
           <t>賴桂蘭</t>
         </is>
       </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>黃素珠</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>楊依如</t>
+          <t>林宏諺</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr">
         <is>
-          <t>吳誼婷</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>鄭靜慧</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr"/>
+          <t>陳怡芯</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>陳彥銘</t>
+        </is>
+      </c>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr">
         <is>
-          <t>陳彥銘, 黃素珠</t>
+          <t>陳昱勳, 陳美娜</t>
         </is>
       </c>
       <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1641,39 +1658,40 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>陳怡芯, 楊依如</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>吳靜蕙</t>
-        </is>
-      </c>
+          <t>賴桂蘭</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>陳美娜</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>陳美娜</t>
+          <t>鄭靜慧</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr">
         <is>
-          <t>黃素珠</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>林宏諺</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr"/>
+          <t>李巧如</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>吳誼婷</t>
+        </is>
+      </c>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr">
         <is>
-          <t>吳誼婷, 賴桂蘭</t>
+          <t>陳怡芯, 黃素珠</t>
         </is>
       </c>
       <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1688,39 +1706,40 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>陳昱勳, 陳美娜</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr">
+          <t>賴桂蘭</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>楊依如</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr">
         <is>
           <t>林宏諺</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>鄭靜慧</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr">
         <is>
-          <t>賴桂蘭</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>楊依如</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr"/>
+          <t>林群皓</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>吳靜蕙</t>
+        </is>
+      </c>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr">
         <is>
-          <t>李巧如, 黃素珠</t>
+          <t>李巧如, 陳美娜</t>
         </is>
       </c>
       <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1733,34 +1752,30 @@
           <t>Tue</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>鄭靜慧, 賴桂蘭</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr">
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
         <is>
           <t>黃素珠</t>
         </is>
       </c>
+      <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
-          <t>黃榮壹</t>
+          <t>林宏諺</t>
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
-          <t>陳美娜</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>吳靜蕙</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr"/>
+          <t>陳彥銘</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>陳昱勳</t>
+        </is>
+      </c>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr">
         <is>
@@ -1768,6 +1783,7 @@
         </is>
       </c>
       <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1782,39 +1798,40 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>吳靜蕙, 賴桂蘭</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>陳美娜</t>
-        </is>
-      </c>
+          <t>黃素珠</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>陳美娜</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
-          <t>陳怡芯</t>
+          <t>陳彥銘</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr">
         <is>
-          <t>李巧如</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>黃素珠</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr"/>
+          <t>吳靜蕙</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>楊依如</t>
+        </is>
+      </c>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr">
         <is>
-          <t>吳誼婷, 楊依如</t>
+          <t>鄭靜慧, 賴桂蘭</t>
         </is>
       </c>
       <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1829,39 +1846,40 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>李巧如</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>林群皓</t>
-        </is>
-      </c>
+          <t>黃素珠</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>賴桂蘭</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
-          <t>陳昱勳</t>
+          <t>吳靜蕙</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>林宏諺</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>陳美娜</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr"/>
+          <t>陳昱勳</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>吳誼婷</t>
+        </is>
+      </c>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr">
         <is>
-          <t>陳彥銘, 黃素珠</t>
+          <t>林宏諺, 陳美娜</t>
         </is>
       </c>
       <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1876,39 +1894,40 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>林宏諺, 賴桂蘭</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>吳誼婷</t>
-        </is>
-      </c>
+          <t>黃素珠</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>陳美娜</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
-          <t>李巧如</t>
+          <t>吳靜蕙</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
-          <t>陳彥銘</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>黃榮壹</t>
-        </is>
-      </c>
-      <c r="J31" t="inlineStr"/>
+          <t>陳怡芯</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>楊依如</t>
+        </is>
+      </c>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr">
         <is>
-          <t>林群皓, 楊依如</t>
+          <t>陳彥銘, 賴桂蘭</t>
         </is>
       </c>
       <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1923,39 +1942,40 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>陳彥銘, 賴桂蘭</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr">
-        <is>
           <t>黃素珠</t>
         </is>
       </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>楊依如</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
-          <t>吳靜蕙</t>
+          <t>陳怡芯</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
-          <t>楊依如</t>
-        </is>
-      </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>陳怡芯</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr"/>
+          <t>吳誼婷</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>鄭靜慧</t>
+        </is>
+      </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr">
         <is>
-          <t>黃榮壹, 陳美娜</t>
+          <t>陳昱勳, 陳美娜</t>
         </is>
       </c>
       <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>